<commit_message>
Finanzas actualizadas, Se ha cambiado almacenamiento de 4tb a 12TB y el RAID 5 pasa ahora a ser RAID 0
</commit_message>
<xml_diff>
--- a/Finanzas/Calculos.xlsx
+++ b/Finanzas/Calculos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luish\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luish\Nextcloud2\Documentos\WorkSpace\CloudStorage_Project\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B1861418-C260-4A63-BF98-05CB7AF6185F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09F40266-E1F5-4E51-B77D-9B30B3E2613E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-2820" windowWidth="24220" windowHeight="16220" xr2:uid="{2ACD9D76-AA8A-4D8B-950C-8B698299ACBF}"/>
   </bookViews>
@@ -16,37 +16,37 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Hoja1!$I$2:$I$6</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Hoja1!$J$2:$J$6</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Hoja1!$I$2</definedName>
-    <definedName name="solver_lhs10" localSheetId="0" hidden="1">Hoja1!$I$5</definedName>
-    <definedName name="solver_lhs11" localSheetId="0" hidden="1">Hoja1!$I$5</definedName>
-    <definedName name="solver_lhs12" localSheetId="0" hidden="1">Hoja1!$I$6</definedName>
-    <definedName name="solver_lhs13" localSheetId="0" hidden="1">Hoja1!$I$6</definedName>
-    <definedName name="solver_lhs14" localSheetId="0" hidden="1">Hoja1!$I$6</definedName>
-    <definedName name="solver_lhs15" localSheetId="0" hidden="1">Hoja1!$I$6</definedName>
-    <definedName name="solver_lhs16" localSheetId="0" hidden="1">Hoja1!$K$17</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Hoja1!$I$2:$I$6</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Hoja1!$I$3</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Hoja1!$I$4</definedName>
-    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Hoja1!$I$5</definedName>
-    <definedName name="solver_lhs6" localSheetId="0" hidden="1">Hoja1!$I$6</definedName>
-    <definedName name="solver_lhs7" localSheetId="0" hidden="1">Hoja1!$I$6</definedName>
-    <definedName name="solver_lhs8" localSheetId="0" hidden="1">Hoja1!$I$6</definedName>
-    <definedName name="solver_lhs9" localSheetId="0" hidden="1">Hoja1!$I$6</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Hoja1!$J$2</definedName>
+    <definedName name="solver_lhs10" localSheetId="0" hidden="1">Hoja1!$J$5</definedName>
+    <definedName name="solver_lhs11" localSheetId="0" hidden="1">Hoja1!$J$5</definedName>
+    <definedName name="solver_lhs12" localSheetId="0" hidden="1">Hoja1!$J$6</definedName>
+    <definedName name="solver_lhs13" localSheetId="0" hidden="1">Hoja1!$J$6</definedName>
+    <definedName name="solver_lhs14" localSheetId="0" hidden="1">Hoja1!$J$6</definedName>
+    <definedName name="solver_lhs15" localSheetId="0" hidden="1">Hoja1!$J$6</definedName>
+    <definedName name="solver_lhs16" localSheetId="0" hidden="1">Hoja1!$J$18</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Hoja1!$J$2:$J$6</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Hoja1!$J$3</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Hoja1!$J$4</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Hoja1!$J$5</definedName>
+    <definedName name="solver_lhs6" localSheetId="0" hidden="1">Hoja1!$J$6</definedName>
+    <definedName name="solver_lhs7" localSheetId="0" hidden="1">Hoja1!$J$18</definedName>
+    <definedName name="solver_lhs8" localSheetId="0" hidden="1">Hoja1!$J$6</definedName>
+    <definedName name="solver_lhs9" localSheetId="0" hidden="1">Hoja1!$J$6</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">6</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">7</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Hoja1!$K$14</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Hoja1!$J$19</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
@@ -65,21 +65,21 @@
     <definedName name="solver_rel7" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel9" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Hoja1!$H$2</definedName>
-    <definedName name="solver_rhs10" localSheetId="0" hidden="1">Hoja1!$H$5</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Hoja1!$I$2</definedName>
+    <definedName name="solver_rhs10" localSheetId="0" hidden="1">Hoja1!$I$5</definedName>
     <definedName name="solver_rhs11" localSheetId="0" hidden="1">"entero"</definedName>
-    <definedName name="solver_rhs12" localSheetId="0" hidden="1">Hoja1!$H$6</definedName>
+    <definedName name="solver_rhs12" localSheetId="0" hidden="1">Hoja1!$I$6</definedName>
     <definedName name="solver_rhs13" localSheetId="0" hidden="1">"entero"</definedName>
     <definedName name="solver_rhs14" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs15" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs16" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">"entero"</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Hoja1!$H$3</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">Hoja1!$H$4</definedName>
-    <definedName name="solver_rhs5" localSheetId="0" hidden="1">Hoja1!$H$5</definedName>
-    <definedName name="solver_rhs6" localSheetId="0" hidden="1">Hoja1!$H$6</definedName>
-    <definedName name="solver_rhs7" localSheetId="0" hidden="1">Hoja1!$H$6</definedName>
-    <definedName name="solver_rhs8" localSheetId="0" hidden="1">Hoja1!$H$6</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Hoja1!$I$3</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">Hoja1!$I$4</definedName>
+    <definedName name="solver_rhs5" localSheetId="0" hidden="1">Hoja1!$I$5</definedName>
+    <definedName name="solver_rhs6" localSheetId="0" hidden="1">Hoja1!$I$6</definedName>
+    <definedName name="solver_rhs7" localSheetId="0" hidden="1">Hoja1!$J$13</definedName>
+    <definedName name="solver_rhs8" localSheetId="0" hidden="1">Hoja1!$I$6</definedName>
     <definedName name="solver_rhs9" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
@@ -89,7 +89,7 @@
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_val" localSheetId="0" hidden="1">330</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -112,8 +112,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Inversion</t>
   </si>
@@ -130,9 +152,6 @@
     <t>cantidad</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>PRECIO/mes</t>
   </si>
   <si>
@@ -157,9 +176,6 @@
     <t>Años para rentabilizar</t>
   </si>
   <si>
-    <t>Almacenamiento (4TB)</t>
-  </si>
-  <si>
     <t>OPTIMO</t>
   </si>
   <si>
@@ -176,6 +192,15 @@
   </si>
   <si>
     <t>DATO</t>
+  </si>
+  <si>
+    <t>Inversion inicial</t>
+  </si>
+  <si>
+    <t>Almacenamiento (12TB)</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -185,18 +210,10 @@
   <numFmts count="3">
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -444,9 +461,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -455,8 +471,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -465,110 +481,37 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="5" tint="0.39997558519241921"/>
@@ -623,6 +566,31 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -637,10 +605,48 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color indexed="64"/>
-        </bottom>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -654,6 +660,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -673,27 +686,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1093AF6-B3F6-4072-8920-3C1491C46620}" name="Tabla1" displayName="Tabla1" ref="E1:I6" totalsRowShown="0" headerRowBorderDxfId="11" tableBorderDxfId="12">
-  <autoFilter ref="E1:I6" xr:uid="{C1093AF6-B3F6-4072-8920-3C1491C46620}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1093AF6-B3F6-4072-8920-3C1491C46620}" name="Tabla1" displayName="Tabla1" ref="F1:J6" totalsRowShown="0" headerRowBorderDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="F1:J6" xr:uid="{C1093AF6-B3F6-4072-8920-3C1491C46620}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0FBF15ED-0AA3-4F15-837C-E2DFF6428927}" name="PRECIO/mes" dataDxfId="4">
-      <calculatedColumnFormula>F2/12</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{0FBF15ED-0AA3-4F15-837C-E2DFF6428927}" name="PRECIO/mes" dataDxfId="10">
+      <calculatedColumnFormula>G2/12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{AE3B3C9E-0048-4C49-A116-F7081B9A4620}" name="Precio/año" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{D89A9E81-CD09-4F1D-BCC5-B186CF7D9027}" name="Almacenamiento(GB)" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{FF7D0B39-C4F4-4F5C-BCF6-453EF24AECED}" name="Maximo usuarios" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{B8E6C0AB-9C78-4AF7-906C-5523BCE2A366}" name="OPTIMO" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{AE3B3C9E-0048-4C49-A116-F7081B9A4620}" name="Precio/año" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{D89A9E81-CD09-4F1D-BCC5-B186CF7D9027}" name="Almacenamiento(GB)" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{FF7D0B39-C4F4-4F5C-BCF6-453EF24AECED}" name="Maximo usuarios" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{B8E6C0AB-9C78-4AF7-906C-5523BCE2A366}" name="OPTIMO" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4449223C-F3D0-40D2-B88F-4C2DA1B19805}" name="Tabla2" displayName="Tabla2" ref="A1:C7" totalsRowShown="0" headerRowBorderDxfId="7" tableBorderDxfId="8">
-  <autoFilter ref="A1:C7" xr:uid="{4449223C-F3D0-40D2-B88F-4C2DA1B19805}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4449223C-F3D0-40D2-B88F-4C2DA1B19805}" name="Tabla2" displayName="Tabla2" ref="B1:D7" totalsRowShown="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
+  <autoFilter ref="B1:D7" xr:uid="{4449223C-F3D0-40D2-B88F-4C2DA1B19805}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1ED079A3-1380-43E2-A70A-A399A41D4A77}" name="Hardware" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{50093091-939B-457F-94A0-CF76D0C4ED31}" name="Inversion" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{1ED079A3-1380-43E2-A70A-A399A41D4A77}" name="Hardware" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{50093091-939B-457F-94A0-CF76D0C4ED31}" name="Inversion" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{32FE7E29-836A-4357-8351-15DF29BC3AEB}" name="cantidad"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -701,10 +714,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2C8BB95F-5AE7-4A1D-A7C2-F1C6AD3011B4}" name="Tabla4" displayName="Tabla4" ref="J12:K18" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="J12:K18" xr:uid="{2C8BB95F-5AE7-4A1D-A7C2-F1C6AD3011B4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2C8BB95F-5AE7-4A1D-A7C2-F1C6AD3011B4}" name="Tabla4" displayName="Tabla4" ref="I12:J19" totalsRowShown="0" tableBorderDxfId="6">
+  <autoFilter ref="I12:J19" xr:uid="{2C8BB95F-5AE7-4A1D-A7C2-F1C6AD3011B4}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EE6D0DBA-8632-4C72-8929-C4B6119B0AF1}" name="Nombre" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{EE6D0DBA-8632-4C72-8929-C4B6119B0AF1}" name="Nombre" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{3543C841-E798-4325-B113-393884574E4A}" name="DATO"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1040,18 +1053,27 @@
   <we:alternateReferences>
     <we:reference id="wa104100404" version="3.0.0.1" store="wa104100404" storeType="OMEX"/>
   </we:alternateReferences>
-  <we:properties/>
-  <we:bindings/>
+  <we:properties>
+    <we:property name="UniqueID" value="&quot;202411181734558225196&quot;"/>
+    <we:property name="MCogAH5CCwwe" value="&quot;&quot;"/>
+    <we:property name="MCogAH5CNwEYB1IQOFAtKQ==" value="&quot;PxcN&quot;"/>
+    <we:property name="MCogAH5CCQ8MPF4M" value="&quot;Sw==&quot;"/>
+    <we:property name="MCogAH5CNwEYB1IQOEMiIg==" value="&quot;S3Z6&quot;"/>
+  </we:properties>
+  <we:bindings>
+    <we:binding id="refEdit" type="matrix" appref="{E0D39740-DBE6-46AE-9D54-130289AE987B}"/>
+    <we:binding id="Worker" type="matrix" appref="{CE4CDCD2-B7F1-45AF-B4EC-D66593990B38}"/>
+  </we:bindings>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </we:webextension>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA7960D-97F2-406C-A5F5-7B123C724D76}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:XFC1048555"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,257 +1081,338 @@
     <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5">
+        <v>94</v>
+      </c>
+      <c r="D2" s="22">
+        <v>1</v>
+      </c>
+      <c r="F2" s="11">
+        <f>G2/12</f>
+        <v>0.25</v>
+      </c>
+      <c r="G2" s="27">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3">
+        <v>50</v>
+      </c>
+      <c r="I2" s="4">
+        <f>PRODUCT(J13/H2 * 1)</f>
+        <v>240</v>
+      </c>
+      <c r="J2" s="13">
         <v>10</v>
       </c>
-      <c r="H1" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5">
+        <v>286</v>
+      </c>
+      <c r="D3" s="22">
         <v>2</v>
       </c>
-      <c r="B2" s="6">
-        <v>94</v>
-      </c>
-      <c r="C2" s="25">
+      <c r="F3" s="12">
+        <f t="shared" ref="F3:F6" si="0">G3/12</f>
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="G3" s="19">
+        <v>5.2</v>
+      </c>
+      <c r="H3" s="10">
+        <v>100</v>
+      </c>
+      <c r="I3" s="9">
+        <f>PRODUCT(J13/H3 * 1)</f>
+        <v>120</v>
+      </c>
+      <c r="J3" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="12">
-        <f>F2/12</f>
-        <v>0.25</v>
-      </c>
-      <c r="F2" s="31">
-        <v>3</v>
-      </c>
-      <c r="G2" s="4">
-        <v>50</v>
-      </c>
-      <c r="H2" s="5">
-        <f>PRODUCT(K13/G2 * 1)</f>
-        <v>160</v>
-      </c>
-      <c r="I2" s="14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="6">
-        <v>125</v>
-      </c>
-      <c r="C3" s="25">
-        <v>3</v>
-      </c>
-      <c r="E3" s="13">
-        <f t="shared" ref="E3:E6" si="0">F3/12</f>
-        <v>0.43333333333333335</v>
-      </c>
-      <c r="F3" s="32">
-        <v>5.2</v>
-      </c>
-      <c r="G3" s="11">
-        <v>100</v>
-      </c>
-      <c r="H3" s="10">
-        <f>PRODUCT(K13/G3 * 1)</f>
-        <v>80</v>
-      </c>
-      <c r="I3" s="15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="C4" s="5">
+        <v>329</v>
+      </c>
+      <c r="D4" s="22">
         <v>1</v>
       </c>
-      <c r="B4" s="6">
-        <v>329</v>
-      </c>
-      <c r="C4" s="25">
-        <v>1</v>
-      </c>
-      <c r="E4" s="12">
+      <c r="F4" s="11">
         <f t="shared" si="0"/>
         <v>1.0825</v>
       </c>
-      <c r="F4" s="33">
+      <c r="G4" s="28">
         <v>12.99</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="3">
         <v>250</v>
       </c>
-      <c r="H4" s="5">
-        <f>PRODUCT(K13/G4 * 1)</f>
-        <v>32</v>
-      </c>
-      <c r="I4" s="14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="I4" s="4">
+        <f>PRODUCT(J13/H4 * 1)</f>
+        <v>48</v>
+      </c>
+      <c r="J4" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6">
+      <c r="C5" s="5">
         <v>85</v>
       </c>
-      <c r="C5" s="26">
+      <c r="D5" s="23">
         <v>1</v>
       </c>
-      <c r="E5" s="13">
+      <c r="F5" s="12">
         <f t="shared" si="0"/>
         <v>2.1666666666666665</v>
       </c>
-      <c r="F5" s="34">
+      <c r="G5" s="29">
         <v>26</v>
       </c>
-      <c r="G5" s="11">
+      <c r="H5" s="10">
         <v>500</v>
       </c>
-      <c r="H5" s="10">
-        <f>PRODUCT(K13/G5 * 1)</f>
-        <v>16</v>
-      </c>
-      <c r="I5" s="15">
-        <v>3</v>
-      </c>
-      <c r="J5" s="21"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="12">
+      <c r="I5" s="9">
+        <f>PRODUCT(J13/H5 * 1)</f>
+        <v>24</v>
+      </c>
+      <c r="J5" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="16"/>
+      <c r="D6" s="25"/>
+      <c r="F6" s="11">
         <f t="shared" si="0"/>
         <v>4.333333333333333</v>
       </c>
-      <c r="F6" s="31">
+      <c r="G6" s="27">
         <v>52</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="3">
         <v>1000</v>
       </c>
-      <c r="H6" s="5">
-        <f>PRODUCT(K13/G6 * 1)</f>
-        <v>8</v>
-      </c>
-      <c r="I6" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="I6" s="4">
+        <f>PRODUCT(J13/H6 * 1)</f>
+        <v>12</v>
+      </c>
+      <c r="J6" s="13">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
-        <f>SUM(PRODUCT(B2:C2)+PRODUCT(B3:C3)+PRODUCT(B4:C4)+PRODUCT(B5:C5))</f>
-        <v>883</v>
-      </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="1"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <f>PRODUCT(D3*12000)/2</f>
+        <v>12000</v>
+      </c>
+      <c r="C7" s="6">
+        <f>SUM(PRODUCT(C2:D2)+PRODUCT(C3:D3)+PRODUCT(C4:D4)+PRODUCT(C5:D5))</f>
+        <v>1080</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
       <c r="J12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="7">
+        <f>B7</f>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J13" s="8" t="s">
+      <c r="J14" s="32">
+        <f>C7</f>
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="8">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J14" s="8" t="s">
+      <c r="J15" s="19">
+        <f>SUM(AVERAGE(G2 * J2) + AVERAGE(G3 * J3) + AVERAGE(G4 * J4) + AVERAGE(G5 * J5) + AVERAGE(G6 * J6))</f>
+        <v>601.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="22">
-        <f>SUM(AVERAGE(F2 * I2) + AVERAGE(F3 * I3) + AVERAGE(F4 * I4) + AVERAGE(F5 * I5) + AVERAGE(F6 * I6))</f>
-        <v>307.35000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K15" s="23">
-        <f>B7/K14</f>
-        <v>2.8729461525947615</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K16" s="24" t="str">
-        <f>IMSUB(K13,K17)</f>
-        <v>2150</v>
-      </c>
-    </row>
-    <row r="17" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G17" s="9"/>
-      <c r="J17" s="8" t="s">
+      <c r="J16" s="20">
+        <f>C7/J15</f>
+        <v>1.7943179930220967</v>
+      </c>
+    </row>
+    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="21" t="str">
+        <f>IMSUB(J13,J18)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F18" s="8"/>
+      <c r="I18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="20">
+        <f>SUM(PRODUCT(H2,J2),PRODUCT(H3,J3),PRODUCT(H4,J4),PRODUCT(H5,J5),PRODUCT(H6,J6))</f>
+        <v>11500</v>
+      </c>
+    </row>
+    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="K17" s="23">
-        <f>SUM(PRODUCT(G2,I2),PRODUCT(G3,I3),PRODUCT(G4,I4),PRODUCT(G5,I5),PRODUCT(G6,I6))</f>
-        <v>5850</v>
-      </c>
-    </row>
-    <row r="18" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="J18" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18" s="36">
+      <c r="J19" s="31">
         <f>SUM(Tabla1[OPTIMO])</f>
-        <v>25</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1048550" spans="16383:16383" x14ac:dyDescent="0.25">
+      <c r="XFC1048550" t="e" cm="1">
+        <f t="array" aca="1" ref="XFC1048550" ca="1">_xludf.Row(solver_opt)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048551" spans="16383:16383" x14ac:dyDescent="0.25">
+      <c r="XFC1048551" t="e" cm="1">
+        <f t="array" aca="1" ref="XFC1048551" ca="1">_xludf.Column(solver_opt)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="1048552" spans="16383:16383" x14ac:dyDescent="0.25">
+      <c r="XFC1048552">
+        <f>solver_num</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1048553" spans="16383:16383" x14ac:dyDescent="0.25">
+      <c r="XFC1048553">
+        <f>solver_typ</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1048554" spans="16383:16383" x14ac:dyDescent="0.25">
+      <c r="XFC1048554">
+        <f>solver_eng</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048555" spans="16383:16383" x14ac:dyDescent="0.25">
+      <c r="XFC1048555">
+        <f>solver_val</f>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
+  <scenarios current="1">
+    <scenario name="200 usuarios" locked="1" count="16" user="Luis Hidalgo Aguilar" comment="Creado por Luis Hidalgo Aguilar el 18/12/2024">
+      <inputCells r="I12" val="Nombre"/>
+      <inputCells r="J12" val="DATO"/>
+      <inputCells r="I13" val="Almacenamiento total GB"/>
+      <inputCells r="J13" val="12000"/>
+      <inputCells r="I14" val="Inversion inicial"/>
+      <inputCells r="J14" val="1350"/>
+      <inputCells r="I15" val="Ingresos anuales"/>
+      <inputCells r="J15" val="698"/>
+      <inputCells r="I16" val="Años para rentabilizar"/>
+      <inputCells r="J16" val="1,93409742120344"/>
+      <inputCells r="I17" val="Almacenamiento_restante(GB)"/>
+      <inputCells r="J17" val="100"/>
+      <inputCells r="I18" val="Almacenamiento_Usado(GB)"/>
+      <inputCells r="J18" val="11900"/>
+      <inputCells r="I19" val="Usuarios totales"/>
+      <inputCells r="J19" val="200"/>
+    </scenario>
+    <scenario name="Usuarios totales" locked="1" count="1" user="Luis Hidalgo Aguilar" comment="Creado por Luis Hidalgo Aguilar el 18/12/2024">
+      <inputCells r="J19" val="200"/>
+    </scenario>
+  </scenarios>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{F7C9EE02-42E1-4005-9D12-6889AFFD525C}">
+      <x15:webExtensions xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x15:webExtension appRef="{E0D39740-DBE6-46AE-9D54-130289AE987B}">
+          <xm:f>Hoja1!1:1048576</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{CE4CDCD2-B7F1-45AF-B4EC-D66593990B38}">
+          <xm:f>Hoja1!XFC1048550:XFD1048575</xm:f>
+        </x15:webExtension>
+      </x15:webExtensions>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>